<commit_message>
Updates dataset and fixes padding
</commit_message>
<xml_diff>
--- a/public/assets/data/oedos.xlsx
+++ b/public/assets/data/oedos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="12480" yWindow="460" windowWidth="10000" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8693" uniqueCount="6135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8812" uniqueCount="6213">
   <si>
     <t>name</t>
   </si>
@@ -18435,6 +18435,240 @@
   </si>
   <si>
     <t>Very late 15th cent. From &lt;a href='/term/saco'&gt;saco&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>agro</t>
+  </si>
+  <si>
+    <t>"field"</t>
+  </si>
+  <si>
+    <t>Very late 16th cent. From Latin &lt;i&gt;ager&lt;/i&gt; 'id.'</t>
+  </si>
+  <si>
+    <t>From Proto-Italic *&lt;i&gt;agro-&lt;/i&gt; 'id.' From Proto-Indo-European *&lt;i&gt;h&lt;sub&gt;2&lt;/sub&gt;eǵ-ro-&lt;/i&gt; 'id.'</t>
+  </si>
+  <si>
+    <t>alumno</t>
+  </si>
+  <si>
+    <t>"student," (archaic) "foster child"</t>
+  </si>
+  <si>
+    <t>Very early 17th cent. From Latin &lt;i&gt;alumnus&lt;/i&gt; "student," but originally "foster child," "nursling."</t>
+  </si>
+  <si>
+    <t>From Proto-Italic *&lt;i&gt;alo-mn-o-&lt;/i&gt; "nourished one." From Proto-Indo-European *&lt;i&gt;h&lt;sub&gt;2&lt;/sub&gt;el-o-mh&lt;sub&gt;1&lt;/sub&gt;no-&lt;/i&gt; "being fed." From a root *&lt;i&gt;h&lt;sub&gt;2&lt;/sub&gt;el-&lt;/i&gt; "to feed."</t>
+  </si>
+  <si>
+    <t>bigote</t>
+  </si>
+  <si>
+    <t>"mustache"</t>
+  </si>
+  <si>
+    <t>Late 15th cent. First recorded as &lt;i&gt;bigot de barva&lt;/i&gt; with &lt;i&gt;-e&lt;/i&gt; later added via anaptyxis. Probably borrowed from Swiss German &lt;i&gt;bî Gott&lt;/i&gt; "by God!," taken from Swiss German mercenaries during the Seige of Granada in 1483 - mercenaries who often sported prominent facial hair (Lapesa 1987). Previous theories hypothesized a borrowing from Old French &lt;i&gt;bigot&lt;/i&gt;, slang for mustachioed Norman soldiers; from the Norman surname &lt;i&gt;Bigot&lt;/i&gt;; or from Old French &lt;i&gt;bigot&lt;/i&gt; "pastry resembling a mustache" (see Corominas 1991; Roberts 2015; Covarrubias 1611 respectively). Lapesa's theory has the benefit of both time and place for the word to enter into Spanish.</t>
+  </si>
+  <si>
+    <t>Also a metaphor for the remnant of drink on the upper lip (cf. English &lt;i&gt;milk mustache&lt;/i&gt;).</t>
+  </si>
+  <si>
+    <t>manzana (1)</t>
+  </si>
+  <si>
+    <t>"apple"</t>
+  </si>
+  <si>
+    <t>12th cent. Old Spanish &lt;i&gt;mazana&lt;/i&gt;. From Vulgar Latin &lt;i&gt;mattiana&lt;/i&gt; 'id.' From Latin &lt;i&gt;mala Mattiana&lt;/i&gt;, a golden apple varietal but lit. "Matian apples." Named after the horticulturist Gaius Matius, friend of Cæsar Agustus, who introduced the technique of clipping trees. &lt;i&gt;Mala&lt;/i&gt; "apples" (singular &lt;i&gt;malum&lt;/i&gt;) was borrowed from Ancient Greek μῆλον ‎(mêlon) "fruit," "tree."</t>
+  </si>
+  <si>
+    <t>manzana (2), manzana de Adán</t>
+  </si>
+  <si>
+    <t>(Latin America) "Adam's apple"</t>
+  </si>
+  <si>
+    <t>From Latin &lt;i&gt;pomum Adami&lt;/i&gt; "Adam's apple," a mistranslation of Hebrew &lt;i&gt;tappuach ha-adam&lt;/i&gt; "man's bump" for "Adam's apple."</t>
+  </si>
+  <si>
+    <t>melón (1)</t>
+  </si>
+  <si>
+    <t>"melon"</t>
+  </si>
+  <si>
+    <t>Very early 15th cent. From Late Latin &lt;i&gt;melonem&lt;/i&gt;, accusative of &lt;i&gt;melo&lt;/i&gt; 'id.,' apocopation of earlier &lt;i&gt;melopeponem&lt;/i&gt; "fruit (in the shape of an apple)." Borrowed from Ancient Greek μηλοπέπων (melopépon) 'id.,' a compound of μῆλον ‎(mêlon) "apple," "stonefruit" (see &lt;a href='/term/manzana-1'&gt;manzana&lt;/a&gt;) and πέπων ‎(pépon) "ripe."</t>
+  </si>
+  <si>
+    <t>From Proto-Indo-European *&lt;i&gt;pek&lt;sup&gt;w&lt;/sup&gt;-&lt;/i&gt; "to cook," the same root behind &lt;a href='/term/cocer'&gt;cocer&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Also as an adjectival denoting awkward or uncomfortable behavior.</t>
+  </si>
+  <si>
+    <t>melón (2), meloncillo</t>
+  </si>
+  <si>
+    <t>"Egyptian mongoose"</t>
+  </si>
+  <si>
+    <t>alfombra (1)</t>
+  </si>
+  <si>
+    <t>"carpet"</t>
+  </si>
+  <si>
+    <t>15th cent. From Andalusian Arabic &lt;i&gt;alḥánbal&lt;/i&gt; "carpet," "Moroccan tapestry."</t>
+  </si>
+  <si>
+    <t>alfombra (2)</t>
+  </si>
+  <si>
+    <t>"rubella," "measles"</t>
+  </si>
+  <si>
+    <t>15th cent. From Andalusian Arabic &lt;i&gt;alḥúmra&lt;/i&gt; "measles."</t>
+  </si>
+  <si>
+    <t>almohada</t>
+  </si>
+  <si>
+    <t>"pillow"</t>
+  </si>
+  <si>
+    <t>Very early 15th cent. From Andalusian Arabic &lt;i&gt;almuḥádda&lt;/i&gt; 'id.'</t>
+  </si>
+  <si>
+    <t>azúcar</t>
+  </si>
+  <si>
+    <t>"sugar"</t>
+  </si>
+  <si>
+    <t>13th cent. From Andalusian Arabic &lt;i&gt;assúkkar&lt;/i&gt; 'id.,' itself borrowed from Greek σάκχαρι (sákhari) 'id.,' earlier σάκχαρ (sákk&lt;sup&gt;h&lt;/sup&gt;ar). A loan from an Indic source, perhaps Pali &lt;i&gt;sakkharā-&lt;/i&gt; 'id.' From Sanskrit &lt;i&gt;śárkarā-&lt;/i&gt; 'id.'</t>
+  </si>
+  <si>
+    <t>chingar</t>
+  </si>
+  <si>
+    <t>(obscene) "to fuck;" (Latin America) "to fail," "to miscarry"</t>
+  </si>
+  <si>
+    <t>19th cent. From Romany &lt;i&gt;chingarár&lt;/i&gt; "to fight." Corominas (1991) is skeptical the Latin American senses of failure derive from the same Romany word, and instead speculates a source in an unknown New World language or languages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;i&gt;Chingarár&lt;/i&gt; is probably from Proto-Indo-European *&lt;i&gt;g&lt;sup&gt;wh&lt;/sup&gt;en-&lt;/i&gt; "to strike" but the exact route is uncertain.</t>
+  </si>
+  <si>
+    <t>cui, cuy</t>
+  </si>
+  <si>
+    <t>"guinea pig"</t>
+  </si>
+  <si>
+    <t>16th cent. Borrowed from Quechua &lt;i&gt;quwi&lt;/i&gt; 'id.'</t>
+  </si>
+  <si>
+    <t>gimnasia</t>
+  </si>
+  <si>
+    <t>"gymnastics"</t>
+  </si>
+  <si>
+    <t>19th cent. Borrowed from Latin &lt;i&gt;gymnasia&lt;/i&gt; "bodily exercises," borrowed from Ancient Greek γῠμνᾰ́σιᾰ (gymnásia) 'id.,' the plural of γυμνάσιον (gumnásion) "gymnasium" (see &lt;a href='/term/gimnasio'&gt;gimnasio&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t>gimnasio</t>
+  </si>
+  <si>
+    <t>"gymnasium"</t>
+  </si>
+  <si>
+    <t>17th cent. Borrowed form Latin &lt;i&gt;gymnasium&lt;/i&gt; 'id.,' itself borrowed from Ancient Greek γυμνάσιον ‎(gumnásion) 'id.' Formed from γυμνός (gumnós) "naked," as exercises were performed nude.</t>
+  </si>
+  <si>
+    <t>From Proto-Indo-European *&lt;i&gt;nog&lt;sup&gt;w&lt;/sup&gt;-no-&lt;/i&gt; 'id.' (whence &lt;a href='/term/nudo-1'&gt;nudo (1)&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t>helado</t>
+  </si>
+  <si>
+    <t>"cold," "ice cream"</t>
+  </si>
+  <si>
+    <t>13th cent. An adjectival from &lt;a href='/term/helar'&gt;helar&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>helar</t>
+  </si>
+  <si>
+    <t>"to freeze"</t>
+  </si>
+  <si>
+    <t>impulso</t>
+  </si>
+  <si>
+    <t>"impulse"</t>
+  </si>
+  <si>
+    <t>Late 15th cent. From Latin &lt;i&gt;impulsus&lt;/i&gt; 'id.,' from &lt;i&gt;impellere&lt;/i&gt; "to push against," "to incite." From &lt;i&gt;in-&lt;/i&gt; "in" (see &lt;a href='/term/in-2-en'&gt;in-&lt;/a&gt;) and &lt;i&gt;pellare&lt;/i&gt; "to drive" (see &lt;a href='/term/pulso'&gt;pulso&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t>nudo (1)</t>
+  </si>
+  <si>
+    <t>"naked"</t>
+  </si>
+  <si>
+    <t>13th cent. From Latin &lt;i&gt;nudus&lt;/i&gt; 'id.'</t>
+  </si>
+  <si>
+    <t>From Proto-Italic *&lt;i&gt;noweþo-&lt;/i&gt; 'id.' From Proto-Indo-European *&lt;i&gt;nog&lt;sup&gt;w&lt;/sup&gt;-od&lt;sup&gt;h&lt;/sup&gt;o-&lt;/i&gt; 'id.,' derived from *&lt;i&gt;nog&lt;sup&gt;w&lt;/sup&gt;s&lt;/i&gt; 'id.'</t>
+  </si>
+  <si>
+    <t>nudo (2)</t>
+  </si>
+  <si>
+    <t>"knot"</t>
+  </si>
+  <si>
+    <t>13th cent. From Vulgar Latin *&lt;i&gt;nudus&lt;/i&gt; 'id.,' from Latin &lt;i&gt;nodus&lt;/i&gt; 'id.' The sound change from &lt;i&gt;-o-&lt;/i&gt; to &lt;i&gt;-u-&lt;/i&gt; is not understood.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Proto-Italic *&lt;i&gt;nōdo-&lt;/i&gt; 'id.' From Proto-Indo-European *&lt;i&gt;neh&lt;sub&gt;3&lt;/sub&gt;-do-&lt;/i&gt; 'id.' </t>
+  </si>
+  <si>
+    <t>prever</t>
+  </si>
+  <si>
+    <t>"to foresee"</t>
+  </si>
+  <si>
+    <t>Early 17th cent. From &lt;a href='/term/pre'&gt;pre-&lt;/a&gt; and &lt;a href='/term/ver'&gt;ver&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>tripa</t>
+  </si>
+  <si>
+    <t>"intestine," "gut"</t>
+  </si>
+  <si>
+    <t>Very early 13th cent. Of unknown origin.</t>
+  </si>
+  <si>
+    <t>zanahoria</t>
+  </si>
+  <si>
+    <t>"carrot"</t>
+  </si>
+  <si>
+    <t>14th cent. Old Spanish &lt;i&gt;çanahoria&lt;/i&gt;, dialectic variant &lt;i&gt;safanòria&lt;/i&gt;. Borrowed from Andalusian Arabic *&lt;i&gt;safunnárya&lt;/i&gt; 'id.,' itself borrowed from Ancient Greek σταφυλίνη ἀγρία (stap&lt;sup&gt;h&lt;/sup&gt;ulíne agría) "wild carrot." σταφυλίνη "carrot" is a diminutive of σταφυλή (stap&lt;sup&gt;h&lt;/sup&gt;ulé) "grape," of unknown origin. ἀγρία, when referring to plants meaning "wild," is from ἀγρός (agrós) "field" (see &lt;a href='/term/agro'&gt;agro&lt;/a&gt;).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14th cent. From Vulgar Latin &lt;i&gt;melonem&lt;/i&gt;, accusative of &lt;i&gt;melo&lt;/i&gt; 'id.' From Latin &lt;i&gt;meles&lt;/i&gt; "badger." Of unknown origin, but compare Welsh &lt;i&gt;bele&lt;/i&gt; "marten." </t>
+  </si>
+  <si>
+    <t>13th cent. From Latin &lt;i&gt;gelare&lt;/i&gt; 'id.,' a verb derived from &lt;i&gt;gelus&lt;/i&gt; "frost" (see &lt;a href='/term/hielo'&gt;hielo&lt;/a&gt;).</t>
   </si>
 </sst>
 </file>
@@ -18980,11 +19214,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1820"/>
+  <dimension ref="A1:J1819"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A591" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J606" sqref="J606"/>
+      <pane ySplit="1" topLeftCell="A1713" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1727" sqref="B1727"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -42749,7 +42983,7 @@
       <c r="I1072" s="5"/>
       <c r="J1072" s="5"/>
     </row>
-    <row r="1073" spans="1:10" ht="409" x14ac:dyDescent="0.2">
+    <row r="1073" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1073" s="12" t="s">
         <v>3891</v>
       </c>
@@ -48505,7 +48739,7 @@
       <c r="I1333" s="5"/>
       <c r="J1333" s="5"/>
     </row>
-    <row r="1334" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="1334" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1334" s="25" t="s">
         <v>4788</v>
       </c>
@@ -56968,278 +57202,409 @@
       <c r="J1716" s="5"/>
     </row>
     <row r="1717" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1717" s="5"/>
-      <c r="B1717" s="5"/>
-      <c r="C1717" s="5"/>
-      <c r="D1717" s="5"/>
-      <c r="E1717" s="5"/>
-      <c r="F1717" s="5"/>
-      <c r="G1717" s="5"/>
-      <c r="H1717" s="5"/>
-      <c r="I1717" s="5"/>
-      <c r="J1717" s="5"/>
+      <c r="A1717" s="5" t="s">
+        <v>6135</v>
+      </c>
+      <c r="B1717" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1717" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1717" s="5" t="s">
+        <v>6136</v>
+      </c>
+      <c r="F1717" s="5" t="s">
+        <v>6137</v>
+      </c>
+      <c r="G1717" s="5" t="s">
+        <v>6138</v>
+      </c>
     </row>
     <row r="1718" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1718" s="5"/>
-      <c r="B1718" s="5"/>
-      <c r="C1718" s="5"/>
-      <c r="D1718" s="5"/>
-      <c r="E1718" s="5"/>
-      <c r="F1718" s="5"/>
-      <c r="G1718" s="5"/>
-      <c r="H1718" s="5"/>
-      <c r="I1718" s="5"/>
-      <c r="J1718" s="5"/>
+      <c r="A1718" s="5" t="s">
+        <v>6139</v>
+      </c>
+      <c r="D1718" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1718" s="5" t="s">
+        <v>6140</v>
+      </c>
+      <c r="F1718" s="5" t="s">
+        <v>6141</v>
+      </c>
+      <c r="G1718" s="5" t="s">
+        <v>6142</v>
+      </c>
     </row>
     <row r="1719" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1719" s="5"/>
-      <c r="B1719" s="5"/>
-      <c r="C1719" s="5"/>
-      <c r="D1719" s="5"/>
-      <c r="E1719" s="5"/>
-      <c r="F1719" s="5"/>
-      <c r="G1719" s="5"/>
-      <c r="H1719" s="5"/>
-      <c r="I1719" s="5"/>
-      <c r="J1719" s="5"/>
+      <c r="A1719" s="5" t="s">
+        <v>6143</v>
+      </c>
+      <c r="B1719" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1719" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1719" s="5" t="s">
+        <v>6144</v>
+      </c>
+      <c r="F1719" s="5" t="s">
+        <v>6145</v>
+      </c>
+      <c r="H1719" s="5" t="s">
+        <v>6146</v>
+      </c>
     </row>
     <row r="1720" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1720" s="5"/>
-      <c r="B1720" s="5"/>
-      <c r="C1720" s="5"/>
-      <c r="D1720" s="5"/>
-      <c r="E1720" s="5"/>
-      <c r="F1720" s="5"/>
-      <c r="G1720" s="5"/>
-      <c r="H1720" s="5"/>
-      <c r="I1720" s="5"/>
-      <c r="J1720" s="5"/>
+      <c r="A1720" s="5" t="s">
+        <v>6147</v>
+      </c>
+      <c r="B1720" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1720" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1720" s="5" t="s">
+        <v>6148</v>
+      </c>
+      <c r="F1720" s="5" t="s">
+        <v>6149</v>
+      </c>
+      <c r="G1720" s="5" t="s">
+        <v>843</v>
+      </c>
     </row>
     <row r="1721" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1721" s="5"/>
-      <c r="B1721" s="5"/>
-      <c r="C1721" s="5"/>
-      <c r="D1721" s="5"/>
-      <c r="E1721" s="5"/>
-      <c r="F1721" s="5"/>
-      <c r="G1721" s="5"/>
-      <c r="H1721" s="5"/>
-      <c r="I1721" s="5"/>
-      <c r="J1721" s="5"/>
+      <c r="A1721" s="5" t="s">
+        <v>6150</v>
+      </c>
+      <c r="B1721" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1721" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1721" s="5" t="s">
+        <v>6151</v>
+      </c>
+      <c r="F1721" s="5" t="s">
+        <v>6152</v>
+      </c>
     </row>
     <row r="1722" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1722" s="5"/>
-      <c r="B1722" s="5"/>
-      <c r="C1722" s="5"/>
-      <c r="D1722" s="5"/>
-      <c r="E1722" s="5"/>
-      <c r="F1722" s="5"/>
-      <c r="G1722" s="5"/>
-      <c r="H1722" s="5"/>
-      <c r="I1722" s="5"/>
-      <c r="J1722" s="5"/>
+      <c r="A1722" s="5" t="s">
+        <v>6153</v>
+      </c>
+      <c r="B1722" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1722" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1722" s="5" t="s">
+        <v>6154</v>
+      </c>
+      <c r="F1722" s="5" t="s">
+        <v>6155</v>
+      </c>
+      <c r="G1722" s="5" t="s">
+        <v>6156</v>
+      </c>
+      <c r="H1722" s="5" t="s">
+        <v>6157</v>
+      </c>
     </row>
     <row r="1723" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1723" s="5"/>
-      <c r="B1723" s="5"/>
-      <c r="C1723" s="5"/>
-      <c r="D1723" s="5"/>
-      <c r="E1723" s="5"/>
-      <c r="F1723" s="5"/>
-      <c r="G1723" s="5"/>
-      <c r="H1723" s="5"/>
-      <c r="I1723" s="5"/>
-      <c r="J1723" s="5"/>
+      <c r="A1723" s="5" t="s">
+        <v>6158</v>
+      </c>
+      <c r="D1723" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1723" s="5" t="s">
+        <v>6159</v>
+      </c>
+      <c r="F1723" s="5" t="s">
+        <v>6211</v>
+      </c>
     </row>
     <row r="1724" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1724" s="5"/>
-      <c r="B1724" s="5"/>
-      <c r="C1724" s="5"/>
-      <c r="D1724" s="5"/>
-      <c r="E1724" s="5"/>
-      <c r="F1724" s="5"/>
-      <c r="G1724" s="5"/>
-      <c r="H1724" s="5"/>
-      <c r="I1724" s="5"/>
-      <c r="J1724" s="5"/>
+      <c r="A1724" s="5" t="s">
+        <v>6160</v>
+      </c>
+      <c r="B1724" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1724" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1724" s="5" t="s">
+        <v>6161</v>
+      </c>
+      <c r="F1724" s="5" t="s">
+        <v>6162</v>
+      </c>
     </row>
     <row r="1725" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1725" s="5"/>
-      <c r="B1725" s="5"/>
-      <c r="C1725" s="5"/>
-      <c r="D1725" s="5"/>
-      <c r="E1725" s="5"/>
-      <c r="F1725" s="5"/>
-      <c r="G1725" s="5"/>
-      <c r="H1725" s="5"/>
-      <c r="I1725" s="5"/>
-      <c r="J1725" s="5"/>
+      <c r="A1725" s="5" t="s">
+        <v>6163</v>
+      </c>
+      <c r="B1725" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1725" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1725" s="5" t="s">
+        <v>6164</v>
+      </c>
+      <c r="F1725" s="5" t="s">
+        <v>6165</v>
+      </c>
     </row>
     <row r="1726" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1726" s="5"/>
-      <c r="B1726" s="5"/>
-      <c r="C1726" s="5"/>
-      <c r="D1726" s="5"/>
-      <c r="E1726" s="5"/>
-      <c r="F1726" s="5"/>
-      <c r="G1726" s="5"/>
-      <c r="H1726" s="5"/>
-      <c r="I1726" s="5"/>
-      <c r="J1726" s="5"/>
+      <c r="A1726" s="5" t="s">
+        <v>6166</v>
+      </c>
+      <c r="B1726" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1726" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1726" s="5" t="s">
+        <v>6167</v>
+      </c>
+      <c r="F1726" s="5" t="s">
+        <v>6168</v>
+      </c>
     </row>
     <row r="1727" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1727" s="5"/>
-      <c r="B1727" s="5"/>
-      <c r="C1727" s="5"/>
-      <c r="D1727" s="5"/>
-      <c r="E1727" s="5"/>
-      <c r="F1727" s="5"/>
-      <c r="G1727" s="5"/>
-      <c r="H1727" s="5"/>
-      <c r="I1727" s="5"/>
-      <c r="J1727" s="5"/>
+      <c r="A1727" s="5" t="s">
+        <v>6169</v>
+      </c>
+      <c r="B1727" s="5" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D1727" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1727" s="5" t="s">
+        <v>6170</v>
+      </c>
+      <c r="F1727" s="5" t="s">
+        <v>6171</v>
+      </c>
     </row>
     <row r="1728" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1728" s="5"/>
-      <c r="B1728" s="5"/>
-      <c r="C1728" s="5"/>
-      <c r="D1728" s="5"/>
-      <c r="E1728" s="5"/>
-      <c r="F1728" s="5"/>
-      <c r="G1728" s="5"/>
-      <c r="H1728" s="5"/>
-      <c r="I1728" s="5"/>
-      <c r="J1728" s="5"/>
-    </row>
-    <row r="1729" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1729" s="5"/>
-      <c r="B1729" s="5"/>
-      <c r="C1729" s="5"/>
-      <c r="D1729" s="5"/>
-      <c r="E1729" s="5"/>
-      <c r="F1729" s="5"/>
-      <c r="G1729" s="5"/>
-      <c r="H1729" s="5"/>
-      <c r="I1729" s="5"/>
-      <c r="J1729" s="5"/>
-    </row>
-    <row r="1730" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1730" s="5"/>
-      <c r="B1730" s="5"/>
-      <c r="C1730" s="5"/>
-      <c r="D1730" s="5"/>
-      <c r="E1730" s="5"/>
-      <c r="F1730" s="5"/>
-      <c r="G1730" s="5"/>
-      <c r="H1730" s="5"/>
-      <c r="I1730" s="5"/>
-      <c r="J1730" s="5"/>
-    </row>
-    <row r="1731" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1731" s="5"/>
-      <c r="B1731" s="5"/>
-      <c r="C1731" s="5"/>
-      <c r="D1731" s="5"/>
-      <c r="E1731" s="5"/>
-      <c r="F1731" s="5"/>
-      <c r="G1731" s="5"/>
-      <c r="H1731" s="5"/>
-      <c r="I1731" s="5"/>
-      <c r="J1731" s="5"/>
-    </row>
-    <row r="1732" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1732" s="5"/>
-      <c r="B1732" s="5"/>
-      <c r="C1732" s="5"/>
-      <c r="D1732" s="5"/>
-      <c r="E1732" s="5"/>
-      <c r="F1732" s="5"/>
-      <c r="G1732" s="5"/>
-      <c r="H1732" s="5"/>
-      <c r="I1732" s="5"/>
-      <c r="J1732" s="5"/>
-    </row>
-    <row r="1733" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1733" s="5"/>
-      <c r="B1733" s="5"/>
-      <c r="C1733" s="5"/>
-      <c r="D1733" s="5"/>
-      <c r="E1733" s="5"/>
-      <c r="F1733" s="5"/>
-      <c r="G1733" s="5"/>
-      <c r="H1733" s="5"/>
-      <c r="I1733" s="5"/>
-      <c r="J1733" s="5"/>
-    </row>
-    <row r="1734" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1734" s="5"/>
-      <c r="B1734" s="5"/>
-      <c r="C1734" s="5"/>
-      <c r="D1734" s="5"/>
-      <c r="E1734" s="5"/>
-      <c r="F1734" s="5"/>
-      <c r="G1734" s="5"/>
-      <c r="H1734" s="5"/>
-      <c r="I1734" s="5"/>
-      <c r="J1734" s="5"/>
-    </row>
-    <row r="1735" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1735" s="5"/>
-      <c r="B1735" s="5"/>
-      <c r="C1735" s="5"/>
-      <c r="D1735" s="5"/>
-      <c r="E1735" s="5"/>
-      <c r="F1735" s="5"/>
-      <c r="G1735" s="5"/>
-      <c r="H1735" s="5"/>
-      <c r="I1735" s="5"/>
-      <c r="J1735" s="5"/>
-    </row>
-    <row r="1736" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1736" s="5"/>
-      <c r="B1736" s="5"/>
-      <c r="C1736" s="5"/>
-      <c r="D1736" s="5"/>
-      <c r="E1736" s="5"/>
-      <c r="F1736" s="5"/>
-      <c r="G1736" s="5"/>
-      <c r="H1736" s="5"/>
-      <c r="I1736" s="5"/>
-      <c r="J1736" s="5"/>
-    </row>
-    <row r="1737" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1737" s="5"/>
-      <c r="B1737" s="5"/>
-      <c r="C1737" s="5"/>
-      <c r="D1737" s="5"/>
-      <c r="E1737" s="5"/>
-      <c r="F1737" s="5"/>
-      <c r="G1737" s="5"/>
-      <c r="H1737" s="5"/>
-      <c r="I1737" s="5"/>
-      <c r="J1737" s="5"/>
-    </row>
-    <row r="1738" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1738" s="5"/>
-      <c r="B1738" s="5"/>
-      <c r="C1738" s="5"/>
-      <c r="D1738" s="5"/>
-      <c r="E1738" s="5"/>
-      <c r="F1738" s="5"/>
-      <c r="G1738" s="5"/>
-      <c r="H1738" s="5"/>
-    </row>
-    <row r="1739" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1739" s="5"/>
-      <c r="B1739" s="5"/>
-      <c r="C1739" s="5"/>
-      <c r="D1739" s="5"/>
-      <c r="E1739" s="5"/>
-      <c r="F1739" s="5"/>
-      <c r="G1739" s="5"/>
-      <c r="H1739" s="5"/>
-    </row>
-    <row r="1740" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1728" s="5" t="s">
+        <v>6172</v>
+      </c>
+      <c r="D1728" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1728" s="5" t="s">
+        <v>6173</v>
+      </c>
+      <c r="F1728" s="5" t="s">
+        <v>6174</v>
+      </c>
+      <c r="G1728" s="5" t="s">
+        <v>6175</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1729" s="5" t="s">
+        <v>6176</v>
+      </c>
+      <c r="B1729" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1729" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1729" s="5" t="s">
+        <v>6177</v>
+      </c>
+      <c r="F1729" s="5" t="s">
+        <v>6178</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1730" s="5" t="s">
+        <v>6179</v>
+      </c>
+      <c r="B1730" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1730" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1730" s="5" t="s">
+        <v>6180</v>
+      </c>
+      <c r="F1730" s="5" t="s">
+        <v>6181</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1731" s="5" t="s">
+        <v>6182</v>
+      </c>
+      <c r="B1731" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1731" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1731" s="5" t="s">
+        <v>6183</v>
+      </c>
+      <c r="F1731" s="5" t="s">
+        <v>6184</v>
+      </c>
+      <c r="G1731" s="5" t="s">
+        <v>6185</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1732" s="5" t="s">
+        <v>6186</v>
+      </c>
+      <c r="B1732" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1732" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1732" s="5" t="s">
+        <v>6187</v>
+      </c>
+      <c r="F1732" s="5" t="s">
+        <v>6188</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1733" s="5" t="s">
+        <v>6189</v>
+      </c>
+      <c r="D1733" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1733" s="5" t="s">
+        <v>6190</v>
+      </c>
+      <c r="F1733" s="5" t="s">
+        <v>6212</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1734" s="5" t="s">
+        <v>6191</v>
+      </c>
+      <c r="B1734" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1734" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1734" s="5" t="s">
+        <v>6192</v>
+      </c>
+      <c r="F1734" s="5" t="s">
+        <v>6193</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1735" s="5" t="s">
+        <v>6194</v>
+      </c>
+      <c r="D1735" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1735" s="5" t="s">
+        <v>6195</v>
+      </c>
+      <c r="F1735" s="5" t="s">
+        <v>6196</v>
+      </c>
+      <c r="G1735" s="5" t="s">
+        <v>6197</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1736" s="5" t="s">
+        <v>6198</v>
+      </c>
+      <c r="B1736" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1736" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1736" s="5" t="s">
+        <v>6199</v>
+      </c>
+      <c r="F1736" s="5" t="s">
+        <v>6200</v>
+      </c>
+      <c r="G1736" s="5" t="s">
+        <v>6201</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1737" s="5" t="s">
+        <v>6202</v>
+      </c>
+      <c r="D1737" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1737" s="5" t="s">
+        <v>6203</v>
+      </c>
+      <c r="F1737" s="5" t="s">
+        <v>6204</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1738" s="5" t="s">
+        <v>6205</v>
+      </c>
+      <c r="B1738" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1738" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1738" s="5" t="s">
+        <v>6206</v>
+      </c>
+      <c r="F1738" s="5" t="s">
+        <v>6207</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1739" s="5" t="s">
+        <v>6208</v>
+      </c>
+      <c r="B1739" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1739" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1739" s="5" t="s">
+        <v>6209</v>
+      </c>
+      <c r="F1739" s="5" t="s">
+        <v>6210</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1740" s="5"/>
       <c r="B1740" s="5"/>
       <c r="C1740" s="5"/>
@@ -57249,7 +57614,7 @@
       <c r="G1740" s="5"/>
       <c r="H1740" s="5"/>
     </row>
-    <row r="1741" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1741" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1741" s="5"/>
       <c r="B1741" s="5"/>
       <c r="C1741" s="5"/>
@@ -57259,7 +57624,7 @@
       <c r="G1741" s="5"/>
       <c r="H1741" s="5"/>
     </row>
-    <row r="1742" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1742" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1742" s="5"/>
       <c r="B1742" s="5"/>
       <c r="C1742" s="5"/>
@@ -57269,7 +57634,7 @@
       <c r="G1742" s="5"/>
       <c r="H1742" s="5"/>
     </row>
-    <row r="1743" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1743" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1743" s="5"/>
       <c r="B1743" s="5"/>
       <c r="C1743" s="5"/>
@@ -57279,7 +57644,7 @@
       <c r="G1743" s="5"/>
       <c r="H1743" s="5"/>
     </row>
-    <row r="1744" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1744" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1744" s="5"/>
       <c r="B1744" s="5"/>
       <c r="C1744" s="5"/>
@@ -58039,16 +58404,6 @@
       <c r="G1819" s="5"/>
       <c r="H1819" s="5"/>
     </row>
-    <row r="1820" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1820" s="5"/>
-      <c r="B1820" s="5"/>
-      <c r="C1820" s="5"/>
-      <c r="D1820" s="5"/>
-      <c r="E1820" s="5"/>
-      <c r="F1820" s="5"/>
-      <c r="G1820" s="5"/>
-      <c r="H1820" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>